<commit_message>
Exported H01 manufactuirng data
</commit_message>
<xml_diff>
--- a/Hardware/TrackJet_H01/BOM.xlsx
+++ b/Hardware/TrackJet_H01/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marou\Projekty\Vedatori\TrackJet\Hardware\TrackJet_H01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C1A8F53-245E-4B58-B010-468C2A815AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB60A09-ABC6-4AAE-A34E-860A8AF0881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{BC484F16-3FC3-4A1A-B915-D2B5F306084F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="169">
   <si>
     <t>Comment</t>
   </si>
@@ -102,30 +102,6 @@
   </si>
   <si>
     <t>C1588</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>C45,C51,C54</t>
-  </si>
-  <si>
-    <t>Capacitor_THT:CP_Radial_D5.0mm_P2.00mm</t>
-  </si>
-  <si>
-    <t>C43803</t>
-  </si>
-  <si>
-    <t>1000u 16V</t>
-  </si>
-  <si>
-    <t>C49,C52,C57</t>
-  </si>
-  <si>
-    <t>Capacitor_THT:CP_Radial_D8.0mm_P3.50mm</t>
-  </si>
-  <si>
-    <t>C43348</t>
   </si>
   <si>
     <t>10u</t>
@@ -965,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240DA6CC-5F1E-4930-9FFB-673C5AC66D83}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F44" si="0">LEN(B2)-LEN(SUBSTITUTE(B2,",",""))+1</f>
+        <f t="shared" ref="F2:F42" si="0">LEN(B2)-LEN(SUBSTITUTE(B2,",",""))+1</f>
         <v>2</v>
       </c>
     </row>
@@ -1116,7 +1092,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,81 +1103,81 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F13">
@@ -1224,7 +1200,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,16 +1223,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1265,16 +1241,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1283,16 +1259,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1301,52 +1277,52 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -1355,16 +1331,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1373,52 +1349,52 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
@@ -1427,16 +1403,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
@@ -1445,124 +1421,124 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -1571,106 +1547,106 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>113</v>
-      </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>126</v>
-      </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -1679,121 +1655,121 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="D42" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="3" t="s">
         <v>142</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="F43:F50" si="1">LEN(B43)-LEN(SUBSTITUTE(B43,",",""))+1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="F44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="F45">
-        <f t="shared" ref="F45:F52" si="1">LEN(B45)-LEN(SUBSTITUTE(B45,",",""))+1</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>153</v>
@@ -1804,35 +1780,35 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
@@ -1841,13 +1817,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>164</v>
@@ -1875,46 +1851,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F55">
-        <f>SUM(F2:F54)</f>
-        <v>162</v>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f>SUM(F2:F52)</f>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed LED colors and indexes.
</commit_message>
<xml_diff>
--- a/Hardware/TrackJet_H01/BOM.xlsx
+++ b/Hardware/TrackJet_H01/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marou\Projekty\Vedatori\TrackJet\Hardware\TrackJet_H01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB20767F-031B-47E1-B42A-D74A5BBEFB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774E1E1-A5E1-4EE2-8C37-5B89222C2D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC484F16-3FC3-4A1A-B915-D2B5F306084F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="173">
   <si>
     <t>Comment</t>
   </si>
@@ -540,6 +540,18 @@
   </si>
   <si>
     <t>C84817</t>
+  </si>
+  <si>
+    <t>U22</t>
+  </si>
+  <si>
+    <t>DRV8833</t>
+  </si>
+  <si>
+    <t>C50506</t>
+  </si>
+  <si>
+    <t>Package_SO:HTSSOP-16-1EP_4.4x5mm_P0.65mm_EP3.4x5mm_Mask2.46x2.31mm_ThermalVias</t>
   </si>
 </sst>
 </file>
@@ -570,7 +582,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -615,11 +627,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -627,6 +648,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -941,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240DA6CC-5F1E-4930-9FFB-673C5AC66D83}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,6 +1676,20 @@
       </c>
       <c r="D50" s="3" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>